<commit_message>
new version of architecture document and sheet
</commit_message>
<xml_diff>
--- a/docs/Smart_city_Fiware_modules_V1.xlsx
+++ b/docs/Smart_city_Fiware_modules_V1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="216">
   <si>
     <t>fiware chapter</t>
   </si>
@@ -166,9 +166,6 @@
   </si>
   <si>
     <t>Wirecloud</t>
-  </si>
-  <si>
-    <t>SpagoBI</t>
   </si>
   <si>
     <t>Freeboard</t>
@@ -909,6 +906,15 @@
     <t>Keystone (OpenStack IDM)
 Horizon (web front end)</t>
   </si>
+  <si>
+    <t>SpagoBI (depredated)</t>
+  </si>
+  <si>
+    <t>web UI, REST API, web integration</t>
+  </si>
+  <si>
+    <t>8000:TCP in use by CKAN =&gt; 8001:TCP ?</t>
+  </si>
 </sst>
 </file>
 
@@ -970,12 +976,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <u/>
       <sz val="11"/>
@@ -984,13 +984,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1006,7 +1024,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1022,11 +1040,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1426,8 +1450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="L32" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Q39" sqref="Q39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1459,7 +1483,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>4</v>
@@ -1483,63 +1507,63 @@
         <v>26</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="O1" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="P1" s="3" t="s">
-        <v>168</v>
-      </c>
       <c r="Q1" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="R1" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>117</v>
       </c>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G4" s="3"/>
     </row>
@@ -1550,28 +1574,28 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G7" s="3"/>
     </row>
@@ -1582,112 +1606,112 @@
     </row>
     <row r="9" spans="1:18" ht="87" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G9" s="3"/>
       <c r="I9" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="116" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>40</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>40</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E11" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q11" s="3" t="s">
         <v>184</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="Q11" s="3" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>40</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
@@ -1697,41 +1721,41 @@
     </row>
     <row r="14" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>164</v>
+        <v>108</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>163</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3" t="s">
         <v>18</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="58" x14ac:dyDescent="0.35">
@@ -1741,38 +1765,38 @@
       <c r="B16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>213</v>
+      <c r="C16" s="8" t="s">
+        <v>212</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>27</v>
       </c>
       <c r="G16" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>108</v>
-      </c>
       <c r="I16" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="58" x14ac:dyDescent="0.35">
@@ -1780,11 +1804,11 @@
         <v>19</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C17" s="7"/>
+        <v>112</v>
+      </c>
+      <c r="C17" s="8"/>
       <c r="D17" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>27</v>
@@ -1793,13 +1817,13 @@
         <v>27</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="58" x14ac:dyDescent="0.35">
@@ -1807,38 +1831,38 @@
         <v>19</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>27</v>
       </c>
       <c r="G18" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="H18" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="H18" s="3" t="s">
-        <v>108</v>
-      </c>
       <c r="I18" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.35">
@@ -1865,28 +1889,28 @@
         <v>12</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>40</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M20" s="3" t="s">
         <v>14</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="29" x14ac:dyDescent="0.35">
@@ -1907,19 +1931,19 @@
         <v>25</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>40</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q21" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="87" x14ac:dyDescent="0.35">
@@ -1931,34 +1955,34 @@
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>40</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N22" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="130.5" x14ac:dyDescent="0.35">
@@ -1970,28 +1994,28 @@
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J23" s="3" t="s">
         <v>40</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q23" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="101.5" x14ac:dyDescent="0.35">
@@ -1999,28 +2023,28 @@
         <v>3</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F24" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="G24" s="3" t="s">
-        <v>153</v>
-      </c>
       <c r="I24" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="Q24" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25" spans="1:17" ht="29" x14ac:dyDescent="0.35">
@@ -2032,19 +2056,19 @@
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="E25" s="5" t="s">
-        <v>102</v>
-      </c>
       <c r="I25" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:17" ht="58" x14ac:dyDescent="0.35">
@@ -2062,25 +2086,25 @@
         <v>36</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J26" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="N26" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="L26" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="N26" s="3" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="29" x14ac:dyDescent="0.35">
@@ -2095,22 +2119,22 @@
         <v>23</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2122,16 +2146,16 @@
         <v>42</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>25</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:17" ht="29" x14ac:dyDescent="0.35">
@@ -2139,29 +2163,29 @@
         <v>3</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="26" customHeight="1" x14ac:dyDescent="0.35">
@@ -2169,11 +2193,11 @@
         <v>3</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G30" s="3"/>
     </row>
@@ -2182,30 +2206,30 @@
         <v>3</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Q31" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="32" spans="1:17" ht="29" x14ac:dyDescent="0.35">
@@ -2214,17 +2238,17 @@
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>88</v>
-      </c>
       <c r="E32" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G32" s="3"/>
       <c r="I32" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:18" ht="29" x14ac:dyDescent="0.35">
@@ -2239,10 +2263,10 @@
         <v>30</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="34" spans="1:18" ht="29" x14ac:dyDescent="0.35">
@@ -2251,10 +2275,10 @@
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>27</v>
@@ -2263,7 +2287,7 @@
         <v>11</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.35">
@@ -2272,10 +2296,10 @@
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>27</v>
@@ -2284,7 +2308,7 @@
         <v>11</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.35">
@@ -2292,11 +2316,11 @@
         <v>29</v>
       </c>
       <c r="B36" s="5"/>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>198</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>199</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>27</v>
@@ -2305,24 +2329,24 @@
         <v>11</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:18" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>204</v>
-      </c>
       <c r="M37" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N37" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:18" ht="29" x14ac:dyDescent="0.35">
@@ -2358,7 +2382,7 @@
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>9</v>
@@ -2367,18 +2391,20 @@
         <v>27</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N39" s="5"/>
       <c r="O39" s="5"/>
       <c r="P39" s="5"/>
-      <c r="Q39" s="5"/>
+      <c r="Q39" s="3" t="s">
+        <v>215</v>
+      </c>
       <c r="R39" s="5"/>
     </row>
     <row r="40" spans="1:18" ht="58" x14ac:dyDescent="0.35">
@@ -2386,23 +2412,23 @@
         <v>33</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E40" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H40" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="H40" s="3" t="s">
+      <c r="I40" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="M40" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="I40" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="M40" s="3" t="s">
-        <v>77</v>
       </c>
       <c r="N40" s="5"/>
       <c r="O40" s="5"/>
@@ -2414,12 +2440,12 @@
       <c r="A41" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B41" s="5" t="s">
-        <v>44</v>
+      <c r="B41" s="10" t="s">
+        <v>213</v>
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>9</v>
@@ -2428,16 +2454,16 @@
         <v>27</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L41" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N41" s="5"/>
       <c r="O41" s="5"/>
@@ -2449,12 +2475,12 @@
       <c r="A42" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="5" t="s">
-        <v>200</v>
+      <c r="B42" s="11" t="s">
+        <v>199</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>9</v>
@@ -2463,16 +2489,19 @@
         <v>27</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>170</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L42" s="3" t="s">
-        <v>71</v>
+        <v>214</v>
       </c>
       <c r="N42" s="5"/>
       <c r="O42" s="5"/>
@@ -2485,23 +2514,23 @@
         <v>33</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="H43" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="E43" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>129</v>
-      </c>
       <c r="I43" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N43" s="5"/>
       <c r="O43" s="5"/>
@@ -2511,7 +2540,7 @@
     </row>
     <row r="44" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>31</v>
@@ -2523,37 +2552,37 @@
     </row>
     <row r="45" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E45" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="H45" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="H45" s="3" t="s">
-        <v>144</v>
-      </c>
       <c r="I45" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B46" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>142</v>
-      </c>
       <c r="E46" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.35">
@@ -2620,7 +2649,7 @@
     <hyperlink ref="B9" r:id="rId40" xr:uid="{86B053B8-8C2D-4B9D-B603-90EE4E0BCB4D}"/>
     <hyperlink ref="C35" r:id="rId41" xr:uid="{1D0091C8-BD19-443F-B72F-28A2DD710C79}"/>
     <hyperlink ref="C36" r:id="rId42" xr:uid="{9BEB3478-A134-4E3A-85DB-E020F7A5DEBB}"/>
-    <hyperlink ref="B41" r:id="rId43" xr:uid="{649CE699-E093-4371-AE1F-252AFD6A080A}"/>
+    <hyperlink ref="B41" r:id="rId43" display="SpagoBI" xr:uid="{649CE699-E093-4371-AE1F-252AFD6A080A}"/>
     <hyperlink ref="B37" r:id="rId44" xr:uid="{442983F8-3430-4E74-B629-A994F3D09C11}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new versions of architecture document and component matrix
</commit_message>
<xml_diff>
--- a/docs/Smart_city_Fiware_modules_V1.xlsx
+++ b/docs/Smart_city_Fiware_modules_V1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="216">
   <si>
     <t>fiware chapter</t>
   </si>
@@ -257,9 +257,6 @@
   </si>
   <si>
     <t>docker or VM or BM ?</t>
-  </si>
-  <si>
-    <t>now Oracle, less performance compared to PostgreSQL</t>
   </si>
   <si>
     <t>need persistent storage volume</t>
@@ -914,6 +911,10 @@
   </si>
   <si>
     <t>8000:TCP in use by CKAN =&gt; 8001:TCP ?</t>
+  </si>
+  <si>
+    <t>now owned by Oracle, 
+less performance compared to PostgreSQL</t>
   </si>
 </sst>
 </file>
@@ -1450,8 +1451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L32" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q39" sqref="Q39"/>
+    <sheetView tabSelected="1" topLeftCell="D19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1462,7 +1463,7 @@
     <col min="4" max="4" width="33.1796875" style="4" customWidth="1"/>
     <col min="5" max="5" width="29.90625" style="3" customWidth="1"/>
     <col min="6" max="6" width="24.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.6328125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="24.1796875" style="4" customWidth="1"/>
     <col min="8" max="9" width="18.26953125" style="3" customWidth="1"/>
     <col min="10" max="10" width="20.7265625" style="3" customWidth="1"/>
     <col min="11" max="11" width="20.90625" style="3" customWidth="1"/>
@@ -1483,7 +1484,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>4</v>
@@ -1507,10 +1508,10 @@
         <v>26</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>49</v>
@@ -1519,51 +1520,51 @@
         <v>7</v>
       </c>
       <c r="O1" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="P1" s="3" t="s">
-        <v>167</v>
-      </c>
       <c r="Q1" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R1" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>116</v>
       </c>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G4" s="3"/>
     </row>
@@ -1574,28 +1575,28 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G7" s="3"/>
     </row>
@@ -1606,112 +1607,112 @@
     </row>
     <row r="9" spans="1:18" ht="87" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G9" s="3"/>
       <c r="I9" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="116" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>40</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>40</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E11" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q11" s="3" t="s">
         <v>183</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="Q11" s="3" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>40</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
@@ -1721,41 +1722,41 @@
     </row>
     <row r="14" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3" t="s">
         <v>18</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="58" x14ac:dyDescent="0.35">
@@ -1766,22 +1767,22 @@
         <v>20</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>27</v>
       </c>
       <c r="G16" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>52</v>
@@ -1790,13 +1791,13 @@
         <v>48</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="58" x14ac:dyDescent="0.35">
@@ -1804,11 +1805,11 @@
         <v>19</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>27</v>
@@ -1817,13 +1818,13 @@
         <v>27</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>52</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="58" x14ac:dyDescent="0.35">
@@ -1831,38 +1832,38 @@
         <v>19</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>27</v>
       </c>
       <c r="G18" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="H18" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>52</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.35">
@@ -1889,7 +1890,7 @@
         <v>12</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>11</v>
@@ -1901,16 +1902,16 @@
         <v>40</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M20" s="3" t="s">
         <v>14</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="29" x14ac:dyDescent="0.35">
@@ -1931,7 +1932,7 @@
         <v>25</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I21" s="3" t="s">
         <v>52</v>
@@ -1940,10 +1941,13 @@
         <v>40</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="Q21" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="87" x14ac:dyDescent="0.35">
@@ -1955,16 +1959,16 @@
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>52</v>
@@ -1973,16 +1977,16 @@
         <v>40</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N22" s="3" t="s">
-        <v>61</v>
+        <v>215</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="130.5" x14ac:dyDescent="0.35">
@@ -1994,28 +1998,31 @@
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J23" s="3" t="s">
         <v>40</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="Q23" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="101.5" x14ac:dyDescent="0.35">
@@ -2023,28 +2030,28 @@
         <v>3</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F24" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="G24" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="I24" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="Q24" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="25" spans="1:17" ht="29" x14ac:dyDescent="0.35">
@@ -2056,19 +2063,19 @@
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="E25" s="5" t="s">
-        <v>101</v>
-      </c>
       <c r="I25" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J25" s="3" t="s">
         <v>59</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:17" ht="58" x14ac:dyDescent="0.35">
@@ -2086,7 +2093,7 @@
         <v>36</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>58</v>
@@ -2095,16 +2102,16 @@
         <v>52</v>
       </c>
       <c r="J26" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="N26" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="L26" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="N26" s="3" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="29" x14ac:dyDescent="0.35">
@@ -2119,7 +2126,7 @@
         <v>23</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>11</v>
@@ -2128,13 +2135,13 @@
         <v>52</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2155,7 +2162,7 @@
         <v>60</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:17" ht="29" x14ac:dyDescent="0.35">
@@ -2173,19 +2180,19 @@
         <v>55</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J29" s="3" t="s">
         <v>54</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="26" customHeight="1" x14ac:dyDescent="0.35">
@@ -2193,11 +2200,11 @@
         <v>3</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G30" s="3"/>
     </row>
@@ -2206,30 +2213,30 @@
         <v>3</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I31" s="5" t="s">
         <v>52</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Q31" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="32" spans="1:17" ht="29" x14ac:dyDescent="0.35">
@@ -2238,13 +2245,13 @@
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="E32" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G32" s="3"/>
       <c r="I32" s="3" t="s">
@@ -2263,10 +2270,10 @@
         <v>30</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="34" spans="1:18" ht="29" x14ac:dyDescent="0.35">
@@ -2275,10 +2282,10 @@
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>27</v>
@@ -2287,7 +2294,7 @@
         <v>11</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.35">
@@ -2296,10 +2303,10 @@
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>27</v>
@@ -2308,7 +2315,7 @@
         <v>11</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.35">
@@ -2317,10 +2324,10 @@
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>197</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>198</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>27</v>
@@ -2329,24 +2336,24 @@
         <v>11</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:18" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>202</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>203</v>
       </c>
       <c r="M37" s="3" t="s">
         <v>56</v>
       </c>
       <c r="N37" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38" spans="1:18" ht="29" x14ac:dyDescent="0.35">
@@ -2397,13 +2404,13 @@
         <v>52</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N39" s="5"/>
       <c r="O39" s="5"/>
       <c r="P39" s="5"/>
       <c r="Q39" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="R39" s="5"/>
     </row>
@@ -2419,16 +2426,16 @@
         <v>46</v>
       </c>
       <c r="E40" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H40" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H40" s="3" t="s">
+      <c r="I40" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="M40" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="I40" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="M40" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="N40" s="5"/>
       <c r="O40" s="5"/>
@@ -2441,11 +2448,11 @@
         <v>33</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>9</v>
@@ -2460,10 +2467,10 @@
         <v>54</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L41" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N41" s="5"/>
       <c r="O41" s="5"/>
@@ -2476,11 +2483,11 @@
         <v>33</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>9</v>
@@ -2492,16 +2499,16 @@
         <v>57</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J42" s="3" t="s">
         <v>54</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L42" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N42" s="5"/>
       <c r="O42" s="5"/>
@@ -2514,23 +2521,23 @@
         <v>33</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="H43" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="E43" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>128</v>
-      </c>
       <c r="I43" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N43" s="5"/>
       <c r="O43" s="5"/>
@@ -2555,17 +2562,17 @@
         <v>47</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E45" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="H45" s="3" t="s">
         <v>142</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>143</v>
       </c>
       <c r="I45" s="3" t="s">
         <v>52</v>
@@ -2576,13 +2583,13 @@
         <v>47</v>
       </c>
       <c r="B46" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>141</v>
-      </c>
       <c r="E46" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
new versions and data traffic estimation
</commit_message>
<xml_diff>
--- a/docs/Smart_city_Fiware_modules_V1.xlsx
+++ b/docs/Smart_city_Fiware_modules_V1.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="227">
   <si>
     <t>fiware chapter</t>
   </si>
@@ -614,6 +614,9 @@
   </si>
   <si>
     <t>part of Cosmos</t>
+  </si>
+  <si>
+    <t>1 GB</t>
   </si>
   <si>
     <t>5050:TCP service port                          8081:TCP API endpoint</t>
@@ -1468,8 +1471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView tabSelected="1" topLeftCell="J24" zoomScale="80" zoomScaleNormal="80" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="14.45"/>
@@ -2148,8 +2151,11 @@
       <c r="N26" s="1" t="s">
         <v>142</v>
       </c>
+      <c r="O26" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="Q26" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="29.1">
@@ -2158,10 +2164,10 @@
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>138</v>
@@ -2173,10 +2179,10 @@
         <v>72</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>100</v>
@@ -2185,7 +2191,7 @@
         <v>142</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="28" spans="1:17" ht="43.5" customHeight="1">
@@ -2194,19 +2200,19 @@
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="8" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>107</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="29" spans="1:17" ht="29.1">
@@ -2214,29 +2220,29 @@
         <v>92</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>97</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="26.1" customHeight="1">
@@ -2244,11 +2250,11 @@
         <v>92</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G30" s="1"/>
     </row>
@@ -2257,30 +2263,30 @@
         <v>92</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I31" s="8" t="s">
         <v>72</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="32" spans="1:17" ht="29.1">
@@ -2289,13 +2295,13 @@
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G32" s="1"/>
       <c r="I32" s="1" t="s">
@@ -2304,32 +2310,32 @@
     </row>
     <row r="33" spans="1:18" ht="29.1">
       <c r="A33" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="34" spans="1:18" ht="29.1">
       <c r="A34" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B34" s="8"/>
       <c r="C34" s="8" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>69</v>
@@ -2338,19 +2344,19 @@
         <v>98</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="35" spans="1:18">
       <c r="A35" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="8" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>69</v>
@@ -2359,19 +2365,19 @@
         <v>98</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="36" spans="1:18">
       <c r="A36" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="9" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>69</v>
@@ -2380,36 +2386,36 @@
         <v>98</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="37" spans="1:18" ht="72.599999999999994">
       <c r="A37" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="38" spans="1:18" ht="29.1">
       <c r="A38" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>137</v>
@@ -2418,22 +2424,22 @@
         <v>69</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="M38" s="8" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="39" spans="1:18" ht="43.5">
       <c r="A39" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>95</v>
@@ -2442,44 +2448,44 @@
         <v>69</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>72</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="N39" s="8"/>
       <c r="O39" s="8"/>
       <c r="P39" s="8"/>
       <c r="Q39" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="R39" s="8"/>
     </row>
     <row r="40" spans="1:18" ht="57.95">
       <c r="A40" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C40" s="8"/>
       <c r="D40" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="N40" s="8"/>
       <c r="O40" s="8"/>
@@ -2489,14 +2495,14 @@
     </row>
     <row r="41" spans="1:18" ht="29.1">
       <c r="A41" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>95</v>
@@ -2505,13 +2511,13 @@
         <v>69</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="L41" s="1" t="s">
         <v>100</v>
@@ -2524,14 +2530,14 @@
     </row>
     <row r="42" spans="1:18" ht="43.5">
       <c r="A42" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>95</v>
@@ -2540,19 +2546,19 @@
         <v>69</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>44</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="N42" s="8"/>
       <c r="O42" s="8"/>
@@ -2562,26 +2568,26 @@
     </row>
     <row r="43" spans="1:18" ht="174">
       <c r="A43" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="N43" s="8"/>
       <c r="O43" s="8"/>
@@ -2591,32 +2597,32 @@
     </row>
     <row r="44" spans="1:18" ht="29.1">
       <c r="A44" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="45" spans="1:18" ht="43.5">
       <c r="A45" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="I45" s="1" t="s">
         <v>72</v>
@@ -2624,16 +2630,16 @@
     </row>
     <row r="46" spans="1:18" ht="43.5">
       <c r="A46" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="47" spans="1:18">

</xml_diff>

<commit_message>
new versions doc archi, schemas, etc...
</commit_message>
<xml_diff>
--- a/docs/Smart_city_Fiware_modules_V1.xlsx
+++ b/docs/Smart_city_Fiware_modules_V1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18822"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18830"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="273">
   <si>
     <t>fiware chapter</t>
   </si>
@@ -70,7 +70,7 @@
     <t>comments</t>
   </si>
   <si>
-    <t>memory usage</t>
+    <t>memory (RAM)</t>
   </si>
   <si>
     <t>docker container 
@@ -151,7 +151,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>2377:TCP</t>
+      <t>2377/TCP</t>
     </r>
     <r>
       <rPr>
@@ -173,7 +173,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>7946:TCP</t>
+      <t>7946/TCP /</t>
     </r>
     <r>
       <rPr>
@@ -183,7 +183,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">/UDP for communication among nodes
+      <t xml:space="preserve">UDP for communication among nodes
 </t>
     </r>
     <r>
@@ -195,7 +195,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>4789:UDP</t>
+      <t>4789/UDP</t>
     </r>
     <r>
       <rPr>
@@ -217,7 +217,7 @@
 take care no docker image building support !</t>
   </si>
   <si>
-    <t>if use FDCS can be secured with Keyrock/Keystone IDM to provide tokens
+    <t>if used FDCS can be secured with Keyrock/Keystone IDM to provide tokens
 and let users to interact with docker on the designed swarm</t>
   </si>
   <si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t>Docker Images Registry</t>
+  </si>
+  <si>
+    <t>through Portus or Gitlab</t>
   </si>
   <si>
     <t>Portus</t>
@@ -268,7 +271,7 @@
     <t>docker service stack</t>
   </si>
   <si>
-    <t>3000:TCP</t>
+    <t>3000/TCP</t>
   </si>
   <si>
     <t>Monitoring</t>
@@ -296,14 +299,14 @@
     <t>web app &amp; RESTful API</t>
   </si>
   <si>
-    <t>min consumption: 4.5mB
-max consumption:</t>
-  </si>
-  <si>
-    <t>33.1MB</t>
-  </si>
-  <si>
-    <t>9000:TCP</t>
+    <t xml:space="preserve">min consumption: 4.5 MB
+</t>
+  </si>
+  <si>
+    <t>33.1 MB</t>
+  </si>
+  <si>
+    <t>9000/TCP</t>
   </si>
   <si>
     <t>prometheus</t>
@@ -315,7 +318,10 @@
     <t>integrated Key-Value DB</t>
   </si>
   <si>
-    <t>9090:TCP</t>
+    <t>Not yet</t>
+  </si>
+  <si>
+    <t>9090/TCP</t>
   </si>
   <si>
     <t>Centreon</t>
@@ -348,6 +354,9 @@
     <t>either a new instance (Docker) or integration to MNCA existing Centreon</t>
   </si>
   <si>
+    <t xml:space="preserve">use existing Centreon </t>
+  </si>
+  <si>
     <t>Security</t>
   </si>
   <si>
@@ -399,14 +408,17 @@
     <t>REST API + web client: Horizon</t>
   </si>
   <si>
-    <t>480 MB</t>
+    <t>1 GB</t>
+  </si>
+  <si>
+    <t>1.16 GB</t>
   </si>
   <si>
     <t>1GB</t>
   </si>
   <si>
-    <t>5000:TCP api public end point
-35357:TCP admin endpoint
+    <t>5000/TCP api public end point
+35357/TCP admin endpoint
 8000 dev web port (80 production)</t>
   </si>
   <si>
@@ -414,19 +426,28 @@
   </si>
   <si>
     <t>Access Control GE (XACML v3.0.  compliant)</t>
+  </si>
+  <si>
+    <t>is element for security</t>
   </si>
   <si>
     <t>files conf &amp; data directories
 to synchronize on instances</t>
   </si>
   <si>
-    <t>4 GB mini</t>
+    <t>Tomcat 7 (java)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 GB </t>
+  </si>
+  <si>
+    <t>836 MB</t>
   </si>
   <si>
     <t>10 GB mini</t>
   </si>
   <si>
-    <t>6019:TCP</t>
+    <t>6019/TCP</t>
   </si>
   <si>
     <t>Pep Proxy</t>
@@ -445,10 +466,13 @@
     <t>100MB</t>
   </si>
   <si>
+    <t>461.3 MB</t>
+  </si>
+  <si>
     <t>250MB</t>
   </si>
   <si>
-    <t>80:TCP</t>
+    <t>80/TCP</t>
   </si>
   <si>
     <t>context &amp; data</t>
@@ -460,7 +484,7 @@
     <t>Context Broker</t>
   </si>
   <si>
-    <t>via Keyrock (Oauth Token)</t>
+    <t>via Keyrock (Oauth2 Token)</t>
   </si>
   <si>
     <t>add instance for query/ take care for subscription</t>
@@ -485,34 +509,51 @@
     <t xml:space="preserve"> better 2 CPU Core</t>
   </si>
   <si>
-    <t>Min 4GB RAM</t>
+    <t>4GB RAM mini</t>
+  </si>
+  <si>
+    <t>257 MB</t>
   </si>
   <si>
     <t>260 MB</t>
   </si>
   <si>
-    <t>1026:TCP</t>
+    <t>1026/TCP</t>
   </si>
   <si>
     <t>NoSQL Database</t>
   </si>
   <si>
+    <t>no need of external access security, internal credentials
+use Docker secrets to secure access password</t>
+  </si>
+  <si>
+    <t>intrinsic, several nodes</t>
+  </si>
+  <si>
+    <t>several Nodes cluster: 3 minimum</t>
+  </si>
+  <si>
+    <t>REST API
+client API sdk for many platforms: java, javascript, ruby, python, .NET</t>
+  </si>
+  <si>
+    <t>mini 4 GB</t>
+  </si>
+  <si>
+    <t>361 MB</t>
+  </si>
+  <si>
+    <t>27017/TCP</t>
+  </si>
+  <si>
+    <t>Mysql</t>
+  </si>
+  <si>
+    <t>SQL database in case it's hard to switch to Postgesql (then citus) a MariaDB &amp; Galera alternative can be used instead</t>
+  </si>
+  <si>
     <t>no need of external access security, internal credentials</t>
-  </si>
-  <si>
-    <t>intrinsic, several nodes</t>
-  </si>
-  <si>
-    <t>several Nodes cluster: 3 minimum</t>
-  </si>
-  <si>
-    <t>27017:TCP</t>
-  </si>
-  <si>
-    <t>Mysql</t>
-  </si>
-  <si>
-    <t>SQL database in case it's hard to switch to Postgesql (then citus) a MariaDB &amp; Galera alternative can be used instead</t>
   </si>
   <si>
     <t>clustering only fail-over with MySQL, but MariaDB can be used with Galera to have a cluster of MySQL compatible database servers</t>
@@ -528,10 +569,10 @@
     <t>need persistent storage volume</t>
   </si>
   <si>
-    <t>now Oracle, less performance compared to PostgreSQL</t>
-  </si>
-  <si>
-    <t>3306:TCP</t>
+    <t>now owned by Oracle, provides lower performance compared to PostgreSQL</t>
+  </si>
+  <si>
+    <t>3306/TCP</t>
   </si>
   <si>
     <t>open source SQL database
@@ -550,14 +591,14 @@
     <t>PAF (PostgreSQL Automatic Failover) : https://github.com/dalibo/PAF/</t>
   </si>
   <si>
-    <t>min consumption: 3.5mB
+    <t>min consumption: 3.5 MB
 max consumption:</t>
   </si>
   <si>
-    <t>286.9 MB</t>
-  </si>
-  <si>
-    <t>5432:TCP</t>
+    <t>287 MB</t>
+  </si>
+  <si>
+    <t>5432/TCP</t>
   </si>
   <si>
     <t>Citus</t>
@@ -609,6 +650,10 @@
   </si>
   <si>
     <t>add instance + LB</t>
+  </si>
+  <si>
+    <t>several instances + LB 
+as a service on a Swarm</t>
   </si>
   <si>
     <r>
@@ -646,7 +691,13 @@
     <t>1 GB RAM</t>
   </si>
   <si>
-    <t>5050:TCP service port                          8081:TCP API endpoint</t>
+    <t>600 MB -&gt; 1 GB</t>
+  </si>
+  <si>
+    <t>10 GB</t>
+  </si>
+  <si>
+    <t>5050/TCP service port                          8081/TCP API endpoint</t>
   </si>
   <si>
     <t>Comet</t>
@@ -661,7 +712,7 @@
     <t>part of cosmos, Orion, Cygnus, databases</t>
   </si>
   <si>
-    <t>8666:TCP</t>
+    <t>8666/TCP</t>
   </si>
   <si>
     <t>Hadoop</t>
@@ -688,16 +739,35 @@
     <t>several instances (Tomcat cluster)</t>
   </si>
   <si>
+    <t>several instances + LB
+need for shared storage to keep engine configuration files</t>
+  </si>
+  <si>
     <t>no</t>
   </si>
   <si>
-    <t>Tomcat (java)</t>
-  </si>
-  <si>
     <t>orion context broker</t>
   </si>
   <si>
-    <t>web app</t>
+    <t>web app for configuration
+REST API for engine</t>
+  </si>
+  <si>
+    <t>8 GB (recommanded)</t>
+  </si>
+  <si>
+    <t>702 MB</t>
+  </si>
+  <si>
+    <t>mini 100 MB</t>
+  </si>
+  <si>
+    <t>8080/TCP
+8686/TCP
+3002/TCP</t>
+  </si>
+  <si>
+    <t>3302/TCP</t>
   </si>
   <si>
     <t>Perseo (Telefonica)</t>
@@ -706,6 +776,12 @@
     <t>Complex Events Processing Telefonica alternative</t>
   </si>
   <si>
+    <t>web UI doesn't work</t>
+  </si>
+  <si>
+    <t>this component won't be used</t>
+  </si>
+  <si>
     <t>CKAN</t>
   </si>
   <si>
@@ -724,7 +800,10 @@
     <t>python application + postgresql database + Solr search tool</t>
   </si>
   <si>
-    <t>8000:TCP</t>
+    <t>984 MB</t>
+  </si>
+  <si>
+    <t>8000/TCP</t>
   </si>
   <si>
     <t>Solr</t>
@@ -734,6 +813,9 @@
   </si>
   <si>
     <t>access through CKAN</t>
+  </si>
+  <si>
+    <t>741 MB</t>
   </si>
   <si>
     <t>IOT</t>
@@ -816,6 +898,45 @@
   </si>
   <si>
     <t>App Mashup</t>
+  </si>
+  <si>
+    <t>via Keyrock (Oauth Token)</t>
+  </si>
+  <si>
+    <t>PostgreSQL (citus cluster)</t>
+  </si>
+  <si>
+    <t>python (2.7) modules among them Django + Nginx</t>
+  </si>
+  <si>
+    <t>841.3 MB</t>
+  </si>
+  <si>
+    <t>8000/TCP in use by CKAN =&gt; 8001/TCP ?</t>
+  </si>
+  <si>
+    <t>Freeboard</t>
+  </si>
+  <si>
+    <t>dashboards from widgets</t>
+  </si>
+  <si>
+    <t>none provided</t>
+  </si>
+  <si>
+    <t>no, js files</t>
+  </si>
+  <si>
+    <t>web server deployment, Docker OK !</t>
+  </si>
+  <si>
+    <t>open source version is just a JS &amp; html library, else a cloud environnement to host dashboards</t>
+  </si>
+  <si>
+    <t>SpagoBI (depredated)</t>
+  </si>
+  <si>
+    <t>Data Viz &amp; BI (Business Intelligence and Big Data Analytics)</t>
   </si>
   <si>
     <r>
@@ -841,34 +962,7 @@
     </r>
   </si>
   <si>
-    <t>python (2.7) modules among them Django + Nginx</t>
-  </si>
-  <si>
-    <t>8000:TCP in use by CKAN =&gt; 8001:TCP ?</t>
-  </si>
-  <si>
-    <t>Freeboard</t>
-  </si>
-  <si>
-    <t>dashboards from widgets</t>
-  </si>
-  <si>
-    <t>none provided</t>
-  </si>
-  <si>
-    <t>no, js files</t>
-  </si>
-  <si>
-    <t>web server deployment, Docker OK !</t>
-  </si>
-  <si>
-    <t>open source version is just a JS &amp; html library, else a cloud environnement to host dashboards</t>
-  </si>
-  <si>
-    <t>SpagoBI (depredated)</t>
-  </si>
-  <si>
-    <t>Data Viz &amp; BI (Business Intelligence and Big Data Analytics)</t>
+    <t>Tomcat (java)</t>
   </si>
   <si>
     <t>CKAN, Orion, any DB</t>
@@ -881,7 +975,16 @@
 SpagoBI evolution</t>
   </si>
   <si>
-    <t>web UI, REST API, web integration</t>
+    <t>web UI, REST API, web integration (javascript SDK)</t>
+  </si>
+  <si>
+    <t>mini: 750 MB</t>
+  </si>
+  <si>
+    <t>2.45 GB</t>
+  </si>
+  <si>
+    <t>default to 8080/TCP conflict with other components</t>
   </si>
   <si>
     <t>Business API Ecosystem - Biz Ecosystem RI</t>
@@ -941,6 +1044,9 @@
     <t>Dev collaboration tools</t>
   </si>
   <si>
+    <t>won't use it</t>
+  </si>
+  <si>
     <t>Eclipse Che</t>
   </si>
   <si>
@@ -951,6 +1057,18 @@
   </si>
   <si>
     <t>Postgresql for multi-tenant management (KeyCloak)</t>
+  </si>
+  <si>
+    <t>min 375 MB</t>
+  </si>
+  <si>
+    <t>494 MB</t>
+  </si>
+  <si>
+    <t>min 179 MB</t>
+  </si>
+  <si>
+    <t>8080/TCP</t>
   </si>
   <si>
     <t>Visual Stdio Code</t>
@@ -1083,7 +1201,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1102,6 +1220,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1261,7 +1382,7 @@
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Interface" dataDxfId="7"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Concerns" dataDxfId="6"/>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="comments" dataDxfId="5"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="memory usage" dataDxfId="4"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="memory (RAM)" dataDxfId="4"/>
     <tableColumn id="17" xr3:uid="{D71B0EF4-7B5D-4708-9087-1AB6E8ACED73}" name="docker container _x000a_image size" dataDxfId="3"/>
     <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="needed storage size" dataDxfId="2"/>
     <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="incoming ports" dataDxfId="1"/>
@@ -1536,9 +1657,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="14.45"/>
@@ -1563,22 +1684,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="29.1">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -1605,7 +1726,7 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="6" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="6" t="s">
@@ -1678,7 +1799,7 @@
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1698,10 +1819,10 @@
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="10"/>
+      <c r="C9" s="11"/>
       <c r="D9" s="1" t="s">
         <v>31</v>
       </c>
@@ -1709,7 +1830,7 @@
       <c r="I9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="R9" s="1" t="s">
+      <c r="R9" s="6" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1717,14 +1838,14 @@
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="11" t="s">
         <v>34</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="6" t="s">
         <v>36</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -1751,1004 +1872,1098 @@
       <c r="D11" s="6" t="s">
         <v>40</v>
       </c>
+      <c r="E11" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="G11" s="1"/>
-      <c r="O11" s="11"/>
+      <c r="O11" s="12"/>
       <c r="P11" s="6"/>
-      <c r="Q11" s="11"/>
+      <c r="Q11" s="12"/>
     </row>
     <row r="12" spans="1:19" ht="43.5">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>41</v>
+      <c r="B12" s="11" t="s">
+        <v>42</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="R12" s="1" t="s">
         <v>48</v>
+      </c>
+      <c r="R12" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="72.599999999999994">
       <c r="A13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" s="10" t="s">
         <v>50</v>
       </c>
+      <c r="B13" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="D13" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>37</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="O13" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="P13" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="R13" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="R13" s="6" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="14" spans="1:19">
-      <c r="B14" s="10"/>
+      <c r="B14" s="11"/>
       <c r="D14" s="1"/>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:19" ht="29.1">
       <c r="A15" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>60</v>
+        <v>50</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>61</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="R15" s="1" t="s">
-        <v>63</v>
+        <v>48</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="R15" s="6" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="72.599999999999994">
       <c r="A16" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" ht="57.95">
+        <v>70</v>
+      </c>
+      <c r="N16" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="57.95">
       <c r="A17" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>70</v>
+        <v>72</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>73</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="O17" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="P17" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="R17" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="57.95">
+      <c r="A18" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q17" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="R17" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" ht="57.95">
-      <c r="A18" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>84</v>
+      <c r="B18" s="11" t="s">
+        <v>88</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>90</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>74</v>
+        <v>77</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>77</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="I18" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="O18" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="P18" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="R18" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="57.95">
+      <c r="A19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="O18" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q18" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="R18" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" ht="57.95">
-      <c r="A19" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="G19" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>94</v>
+        <v>101</v>
+      </c>
+      <c r="P19" s="6" t="s">
+        <v>102</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="R19" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18">
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
+        <v>103</v>
+      </c>
+      <c r="R19" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
       <c r="D20" s="1"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:18" ht="66.95" customHeight="1">
+    <row r="21" spans="1:19" ht="66.95" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="C21" s="10"/>
+        <v>105</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" s="11"/>
       <c r="D21" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>100</v>
+        <v>107</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>108</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>37</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="L21" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="N21" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="O21" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="P21" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="R21" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="72.599999999999994">
+      <c r="A22" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="M21" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="N21" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="O21" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q21" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="R21" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" ht="29.1">
-      <c r="A22" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C22" s="10"/>
+      <c r="B22" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C22" s="11"/>
       <c r="D22" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>112</v>
+        <v>120</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>121</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L22" s="1" t="s">
+      <c r="L22" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="O22" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="P22" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="R22" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="87">
+      <c r="A23" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="R22" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" ht="87">
-      <c r="A23" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="C23" s="10"/>
+      <c r="B23" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="C23" s="11"/>
       <c r="D23" s="1" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>118</v>
+        <v>130</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>131</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>37</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="R23" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" ht="130.5">
+        <v>134</v>
+      </c>
+      <c r="N23" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="R23" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="130.5">
       <c r="A24" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" s="10"/>
+        <v>105</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="11"/>
       <c r="D24" s="1" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>37</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="O24" s="6" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="P24" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="R24" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" ht="101.45">
+        <v>142</v>
+      </c>
+      <c r="R24" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" ht="101.45">
       <c r="A25" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>132</v>
+        <v>105</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>145</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="R25" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" ht="29.1">
+        <v>149</v>
+      </c>
+      <c r="R25" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" ht="29.1">
       <c r="A26" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="C26" s="10"/>
+        <v>105</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="C26" s="11"/>
       <c r="D26" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>139</v>
+        <v>151</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>152</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" ht="57.95">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" ht="57.95">
       <c r="A27" s="1" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B27" s="1"/>
-      <c r="C27" s="10" t="s">
-        <v>143</v>
+      <c r="C27" s="11" t="s">
+        <v>156</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>146</v>
+        <v>159</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>160</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="J27" s="10" t="s">
-        <v>148</v>
+        <v>80</v>
+      </c>
+      <c r="J27" s="11" t="s">
+        <v>162</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>149</v>
+        <v>163</v>
       </c>
       <c r="L27" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="O27" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="P27" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q27" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="R27" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" ht="29.1">
+      <c r="A28" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="N27" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="O27" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="P27" s="6"/>
-      <c r="R27" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" ht="29.1">
-      <c r="A28" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="B28" s="1"/>
-      <c r="C28" s="10" t="s">
-        <v>153</v>
+      <c r="C28" s="11" t="s">
+        <v>169</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>154</v>
+        <v>170</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="L28" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="R28" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" ht="43.5" customHeight="1">
+      <c r="A29" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="N28" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="R28" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" ht="43.5" customHeight="1">
-      <c r="A29" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="B29" s="1"/>
-      <c r="C29" s="10" t="s">
-        <v>158</v>
+      <c r="C29" s="11" t="s">
+        <v>174</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>160</v>
+        <v>176</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>161</v>
+        <v>177</v>
       </c>
       <c r="N29" s="6" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" ht="29.1">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" ht="43.5">
       <c r="A30" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="C30" s="10"/>
+        <v>105</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="C30" s="11"/>
       <c r="D30" s="1" t="s">
-        <v>164</v>
+        <v>180</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>102</v>
+        <v>181</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>182</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>167</v>
+        <v>183</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>92</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="L30" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" ht="26.1" customHeight="1">
+        <v>184</v>
+      </c>
+      <c r="L30" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="O30" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="P30" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q30" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="R30" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="S30" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" ht="26.1" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="C31" s="10"/>
+        <v>105</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="C31" s="11"/>
       <c r="D31" s="1" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="1:18" ht="43.5">
+      <c r="M31" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="N31" s="6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" ht="43.5">
       <c r="A32" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="C32" s="10"/>
+        <v>105</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="C32" s="11"/>
       <c r="D32" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>174</v>
+        <v>196</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>197</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>175</v>
+        <v>198</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="I32" s="10" t="s">
-        <v>77</v>
+        <v>199</v>
+      </c>
+      <c r="I32" s="11" t="s">
+        <v>80</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>177</v>
+        <v>200</v>
+      </c>
+      <c r="P32" s="6" t="s">
+        <v>201</v>
       </c>
       <c r="R32" s="1" t="s">
-        <v>178</v>
+        <v>202</v>
       </c>
     </row>
     <row r="33" spans="1:19" ht="29.1">
       <c r="A33" s="1" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B33" s="1"/>
-      <c r="C33" s="10" t="s">
-        <v>179</v>
+      <c r="C33" s="11" t="s">
+        <v>203</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>180</v>
+        <v>204</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>181</v>
+        <v>205</v>
       </c>
       <c r="G33" s="1"/>
       <c r="I33" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
+      </c>
+      <c r="P33" s="6" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="34" spans="1:19" ht="29.1">
       <c r="A34" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="C34" s="10"/>
+        <v>207</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="C34" s="11"/>
       <c r="D34" s="1" t="s">
-        <v>184</v>
+        <v>209</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>185</v>
+        <v>210</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>186</v>
+        <v>211</v>
       </c>
     </row>
     <row r="35" spans="1:19" ht="29.1">
       <c r="A35" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10" t="s">
-        <v>187</v>
+        <v>207</v>
+      </c>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11" t="s">
+        <v>212</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>188</v>
+        <v>213</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>186</v>
+        <v>211</v>
       </c>
     </row>
     <row r="36" spans="1:19">
       <c r="A36" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10" t="s">
-        <v>189</v>
+        <v>207</v>
+      </c>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11" t="s">
+        <v>214</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>190</v>
+        <v>215</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
     </row>
     <row r="37" spans="1:19">
       <c r="A37" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B37" s="10"/>
-      <c r="C37" s="12" t="s">
-        <v>191</v>
+        <v>207</v>
+      </c>
+      <c r="B37" s="11"/>
+      <c r="C37" s="13" t="s">
+        <v>216</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>192</v>
+        <v>217</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
     </row>
     <row r="38" spans="1:19" ht="72.599999999999994">
       <c r="A38" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>194</v>
+        <v>218</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>219</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>195</v>
+        <v>220</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>196</v>
+        <v>221</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>197</v>
+        <v>222</v>
       </c>
     </row>
     <row r="39" spans="1:19" ht="29.1">
       <c r="A39" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="C39" s="10"/>
+        <v>223</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="C39" s="11"/>
       <c r="D39" s="1" t="s">
-        <v>200</v>
+        <v>225</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="M39" s="10" t="s">
-        <v>202</v>
+        <v>226</v>
+      </c>
+      <c r="M39" s="11" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="40" spans="1:19" ht="43.5">
       <c r="A40" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="C40" s="10"/>
+        <v>223</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="C40" s="11"/>
       <c r="D40" s="1" t="s">
-        <v>204</v>
+        <v>229</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>100</v>
+        <v>230</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>205</v>
+        <v>77</v>
+      </c>
+      <c r="H40" s="9" t="s">
+        <v>231</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="N40" s="10"/>
-      <c r="O40" s="10"/>
-      <c r="P40" s="10"/>
-      <c r="Q40" s="10"/>
+        <v>232</v>
+      </c>
+      <c r="N40" s="11"/>
+      <c r="O40" s="11"/>
+      <c r="P40" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q40" s="11"/>
       <c r="R40" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="S40" s="10"/>
+        <v>234</v>
+      </c>
+      <c r="S40" s="11"/>
     </row>
     <row r="41" spans="1:19" ht="57.95">
       <c r="A41" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="C41" s="10"/>
+        <v>223</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="C41" s="11"/>
       <c r="D41" s="1" t="s">
-        <v>209</v>
+        <v>236</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="I41" s="10" t="s">
-        <v>212</v>
+        <v>237</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="I41" s="11" t="s">
+        <v>239</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="N41" s="10"/>
-      <c r="O41" s="10"/>
-      <c r="P41" s="10"/>
-      <c r="Q41" s="10"/>
-      <c r="R41" s="10"/>
-      <c r="S41" s="10"/>
+        <v>240</v>
+      </c>
+      <c r="N41" s="11"/>
+      <c r="O41" s="11"/>
+      <c r="P41" s="11"/>
+      <c r="Q41" s="11"/>
+      <c r="R41" s="11"/>
+      <c r="S41" s="11"/>
     </row>
     <row r="42" spans="1:19" ht="29.1">
       <c r="A42" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B42" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="C42" s="10"/>
+        <v>223</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="C42" s="11"/>
       <c r="D42" s="1" t="s">
-        <v>215</v>
+        <v>242</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>100</v>
+        <v>230</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>205</v>
+        <v>243</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>167</v>
+        <v>244</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>216</v>
+        <v>245</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="N42" s="10"/>
-      <c r="O42" s="10"/>
-      <c r="P42" s="10"/>
-      <c r="Q42" s="10"/>
-      <c r="R42" s="10"/>
-      <c r="S42" s="10"/>
+        <v>113</v>
+      </c>
+      <c r="N42" s="11"/>
+      <c r="O42" s="11"/>
+      <c r="P42" s="11"/>
+      <c r="Q42" s="11"/>
+      <c r="R42" s="11"/>
+      <c r="S42" s="11"/>
     </row>
     <row r="43" spans="1:19" ht="43.5">
       <c r="A43" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B43" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="C43" s="10"/>
+        <v>223</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="C43" s="11"/>
       <c r="D43" s="1" t="s">
-        <v>218</v>
+        <v>247</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>100</v>
+        <v>230</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>205</v>
+        <v>243</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>167</v>
+        <v>244</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="L43" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="N43" s="10"/>
-      <c r="O43" s="10"/>
-      <c r="P43" s="10"/>
-      <c r="Q43" s="10"/>
-      <c r="R43" s="10"/>
-      <c r="S43" s="10"/>
+        <v>245</v>
+      </c>
+      <c r="L43" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="N43" s="11"/>
+      <c r="O43" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="P43" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q43" s="11"/>
+      <c r="R43" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="S43" s="11"/>
     </row>
     <row r="44" spans="1:19" ht="174">
       <c r="A44" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="C44" s="10"/>
-      <c r="D44" s="10" t="s">
-        <v>221</v>
+        <v>223</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11" t="s">
+        <v>253</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>222</v>
+        <v>254</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>223</v>
+        <v>255</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>224</v>
+        <v>256</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="N44" s="10"/>
-      <c r="O44" s="10"/>
-      <c r="P44" s="10"/>
-      <c r="Q44" s="10"/>
-      <c r="R44" s="10"/>
-      <c r="S44" s="10"/>
+        <v>257</v>
+      </c>
+      <c r="N44" s="11"/>
+      <c r="O44" s="11"/>
+      <c r="P44" s="11"/>
+      <c r="Q44" s="11"/>
+      <c r="R44" s="11"/>
+      <c r="S44" s="11"/>
     </row>
     <row r="45" spans="1:19" ht="29.1">
       <c r="A45" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="B45" s="10" t="s">
-        <v>227</v>
-      </c>
-      <c r="C45" s="10"/>
+        <v>258</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="C45" s="11"/>
       <c r="D45" s="1" t="s">
-        <v>228</v>
+        <v>260</v>
+      </c>
+      <c r="N45" s="6" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="46" spans="1:19" ht="43.5">
       <c r="A46" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="B46" s="10" t="s">
-        <v>229</v>
-      </c>
-      <c r="C46" s="10"/>
+        <v>258</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="C46" s="11"/>
       <c r="D46" s="1" t="s">
-        <v>230</v>
+        <v>263</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>231</v>
+        <v>264</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>232</v>
+        <v>265</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
+      </c>
+      <c r="O46" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="P46" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="Q46" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="R46" s="6" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="47" spans="1:19" ht="43.5">
       <c r="A47" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="B47" s="10" t="s">
-        <v>233</v>
+        <v>258</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>270</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>234</v>
+        <v>271</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>235</v>
+        <v>272</v>
       </c>
     </row>
     <row r="48" spans="1:19">
@@ -2818,11 +3033,12 @@
     <hyperlink ref="B42" r:id="rId43" display="SpagoBI" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
     <hyperlink ref="B38" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
     <hyperlink ref="B11" r:id="rId45" xr:uid="{8A8D59FF-773A-4DCE-AA54-3A9635FD2929}"/>
+    <hyperlink ref="O30" r:id="rId46" xr:uid="{1BD38749-9B8E-4D3C-B377-34495CE50767}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId46"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId47"/>
   <tableParts count="1">
-    <tablePart r:id="rId47"/>
+    <tablePart r:id="rId48"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new versions of docs
</commit_message>
<xml_diff>
--- a/docs/Smart_city_Fiware_modules_V1.xlsx
+++ b/docs/Smart_city_Fiware_modules_V1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18903"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="277">
   <si>
     <t>fiware chapter</t>
   </si>
@@ -107,7 +107,7 @@
     <t>Network</t>
   </si>
   <si>
-    <t>*</t>
+    <t>VMWare</t>
   </si>
   <si>
     <t>virtualisation</t>
@@ -481,6 +481,10 @@
     <t>Orion</t>
   </si>
   <si>
+    <t>Rush (notification relayer)
+queuing module to reduce load for notifications</t>
+  </si>
+  <si>
     <t>Context Broker</t>
   </si>
   <si>
@@ -551,9 +555,6 @@
   </si>
   <si>
     <t>SQL database in case it's hard to switch to Postgesql (then citus) a MariaDB &amp; Galera alternative can be used instead</t>
-  </si>
-  <si>
-    <t>no need of external access security, internal credentials</t>
   </si>
   <si>
     <t>clustering only fail-over with MySQL, but MariaDB can be used with Galera to have a cluster of MySQL compatible database servers</t>
@@ -578,11 +579,6 @@
     <t>open source SQL database
 offers very close performance to Oracle Database compared to MySQL for pure SQL use
 with an easier management layer, very low TCO, used by many organisations.</t>
-  </si>
-  <si>
-    <t>no need of external access security, internal credentials
-but Master Data Management should be worth thinking about to secure globally access from client applications to platform database
-this includes SQL and NoSQL database as well as Hadoop deployments</t>
   </si>
   <si>
     <t>clustering solutions repmgr, pgpool or Citus + docker swarm</t>
@@ -753,7 +749,7 @@
 REST API for engine</t>
   </si>
   <si>
-    <t>8 GB (recommanded)</t>
+    <t>8 GB (recommended)</t>
   </si>
   <si>
     <t>702 MB</t>
@@ -909,6 +905,9 @@
     <t>python (2.7) modules among them Django + Nginx</t>
   </si>
   <si>
+    <t>1 GB recommanded</t>
+  </si>
+  <si>
     <t>841.3 MB</t>
   </si>
   <si>
@@ -930,7 +929,7 @@
     <t>web server deployment, Docker OK !</t>
   </si>
   <si>
-    <t>open source version is just a JS &amp; html library, else a cloud environnement to host dashboards</t>
+    <t>open source version is just a JS &amp; html library, else a cloud environnement is available to host dashboards</t>
   </si>
   <si>
     <t>SpagoBI (depredated)</t>
@@ -1033,6 +1032,19 @@
     <t>Java 8
 Glassfish 4.1
 MySQL 5.5</t>
+  </si>
+  <si>
+    <t>CKAN, Wirecloud</t>
+  </si>
+  <si>
+    <t>TM Forum API
+Web application</t>
+  </si>
+  <si>
+    <t>1 GB min 2 GB recommended</t>
+  </si>
+  <si>
+    <t>2.1 GB</t>
   </si>
   <si>
     <t>Dev &amp; Collaboration tools</t>
@@ -1657,9 +1669,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="14.45"/>
@@ -1787,7 +1799,7 @@
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="6" t="s">
         <v>26</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -2146,28 +2158,30 @@
       <c r="D20" s="1"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:19" ht="66.95" customHeight="1">
+    <row r="21" spans="1:19" ht="89.45" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>105</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="C21" s="11"/>
+      <c r="C21" s="6" t="s">
+        <v>107</v>
+      </c>
       <c r="D21" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>80</v>
@@ -2176,28 +2190,28 @@
         <v>37</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="N21" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="O21" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="P21" s="6" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="R21" s="6" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:19" ht="72.599999999999994">
@@ -2205,20 +2219,20 @@
         <v>105</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>80</v>
@@ -2227,16 +2241,16 @@
         <v>37</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="O22" s="6" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="P22" s="6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="R22" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="87">
@@ -2244,14 +2258,14 @@
         <v>105</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E23" s="1" t="s">
         <v>130</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>122</v>
       </c>
       <c r="F23" s="11" t="s">
         <v>131</v>
@@ -2278,7 +2292,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="130.5">
+    <row r="24" spans="1:19" ht="101.45">
       <c r="A24" s="1" t="s">
         <v>105</v>
       </c>
@@ -2289,14 +2303,14 @@
       <c r="D24" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>48</v>
@@ -2308,13 +2322,13 @@
         <v>133</v>
       </c>
       <c r="O24" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="P24" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="P24" s="6" t="s">
+      <c r="R24" s="6" t="s">
         <v>142</v>
-      </c>
-      <c r="R24" s="6" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="25" spans="1:19" ht="101.45">
@@ -2322,28 +2336,34 @@
         <v>105</v>
       </c>
       <c r="B25" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="D25" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G25" s="1" t="s">
-        <v>148</v>
+      <c r="H25" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>48</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="R25" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" spans="1:19" ht="29.1">
@@ -2351,23 +2371,23 @@
         <v>105</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E26" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="I26" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="J26" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="L26" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="27" spans="1:19" ht="57.95">
@@ -2376,49 +2396,49 @@
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="G27" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="H27" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>161</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>80</v>
       </c>
       <c r="J27" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="K27" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="K27" s="1" t="s">
+      <c r="L27" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="N27" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="L27" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="N27" s="1" t="s">
+      <c r="O27" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="O27" s="6" t="s">
+      <c r="P27" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="P27" s="6" t="s">
+      <c r="Q27" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="Q27" s="6" t="s">
+      <c r="R27" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="R27" s="1" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="28" spans="1:19" ht="29.1">
@@ -2427,34 +2447,34 @@
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>170</v>
-      </c>
       <c r="F28" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>80</v>
       </c>
       <c r="J28" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="K28" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="K28" s="1" t="s">
+      <c r="L28" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="R28" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="N28" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="R28" s="1" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="29" spans="1:19" ht="43.5" customHeight="1">
@@ -2463,22 +2483,22 @@
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="F29" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I29" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I29" s="1" t="s">
+      <c r="K29" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="K29" s="1" t="s">
+      <c r="N29" s="6" t="s">
         <v>177</v>
-      </c>
-      <c r="N29" s="6" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="30" spans="1:19" ht="43.5">
@@ -2486,20 +2506,20 @@
         <v>105</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="G30" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="G30" s="6" t="s">
+      <c r="H30" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="I30" s="6" t="s">
         <v>48</v>
@@ -2508,25 +2528,25 @@
         <v>92</v>
       </c>
       <c r="K30" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="L30" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="L30" s="6" t="s">
+      <c r="O30" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="O30" s="7" t="s">
+      <c r="P30" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="P30" s="6" t="s">
+      <c r="Q30" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="Q30" s="6" t="s">
+      <c r="R30" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="R30" s="6" t="s">
+      <c r="S30" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="S30" s="6" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="31" spans="1:19" ht="26.1" customHeight="1">
@@ -2534,18 +2554,18 @@
         <v>105</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C31" s="11"/>
       <c r="D31" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G31" s="1"/>
       <c r="M31" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="N31" s="6" t="s">
         <v>193</v>
-      </c>
-      <c r="N31" s="6" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="32" spans="1:19" ht="43.5">
@@ -2553,33 +2573,33 @@
         <v>105</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E32" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="F32" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>198</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I32" s="11" t="s">
         <v>80</v>
       </c>
       <c r="J32" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="P32" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="P32" s="6" t="s">
+      <c r="R32" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="R32" s="1" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="33" spans="1:19" ht="29.1">
@@ -2588,176 +2608,180 @@
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>205</v>
       </c>
       <c r="G33" s="1"/>
       <c r="I33" s="1" t="s">
         <v>80</v>
       </c>
       <c r="P33" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="34" spans="1:19" ht="29.1">
       <c r="A34" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B34" s="11" t="s">
         <v>207</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>208</v>
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="K34" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="K34" s="1" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="35" spans="1:19" ht="29.1">
       <c r="A35" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B35" s="11"/>
       <c r="C35" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>213</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>77</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="36" spans="1:19">
       <c r="A36" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B36" s="11"/>
       <c r="C36" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>215</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>77</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="37" spans="1:19">
       <c r="A37" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B37" s="11"/>
       <c r="C37" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>77</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="38" spans="1:19" ht="72.599999999999994">
       <c r="A38" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B38" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="D38" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="M38" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="M38" s="1" t="s">
+      <c r="N38" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="N38" s="1" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="39" spans="1:19" ht="29.1">
       <c r="A39" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B39" s="11" t="s">
         <v>223</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>224</v>
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>77</v>
       </c>
       <c r="J39" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="M39" s="11" t="s">
         <v>226</v>
-      </c>
-      <c r="M39" s="11" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="40" spans="1:19" ht="43.5">
       <c r="A40" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C40" s="11"/>
       <c r="D40" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>230</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>77</v>
       </c>
       <c r="H40" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>80</v>
       </c>
       <c r="J40" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="N40" s="11"/>
+      <c r="O40" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="N40" s="11"/>
-      <c r="O40" s="11"/>
       <c r="P40" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="Q40" s="11"/>
+      <c r="Q40" s="1" t="s">
+        <v>166</v>
+      </c>
       <c r="R40" s="1" t="s">
         <v>234</v>
       </c>
@@ -2765,7 +2789,7 @@
     </row>
     <row r="41" spans="1:19" ht="57.95">
       <c r="A41" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B41" s="11" t="s">
         <v>235</v>
@@ -2783,7 +2807,7 @@
       <c r="I41" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="M41" s="1" t="s">
+      <c r="M41" s="6" t="s">
         <v>240</v>
       </c>
       <c r="N41" s="11"/>
@@ -2795,7 +2819,7 @@
     </row>
     <row r="42" spans="1:19" ht="29.1">
       <c r="A42" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B42" s="14" t="s">
         <v>241</v>
@@ -2805,7 +2829,7 @@
         <v>242</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>77</v>
@@ -2820,7 +2844,7 @@
         <v>245</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N42" s="11"/>
       <c r="O42" s="11"/>
@@ -2831,7 +2855,7 @@
     </row>
     <row r="43" spans="1:19" ht="43.5">
       <c r="A43" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B43" s="15" t="s">
         <v>246</v>
@@ -2841,7 +2865,7 @@
         <v>247</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>77</v>
@@ -2876,7 +2900,7 @@
     </row>
     <row r="44" spans="1:19" ht="174">
       <c r="A44" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B44" s="11" t="s">
         <v>252</v>
@@ -2897,73 +2921,83 @@
       <c r="J44" s="1" t="s">
         <v>257</v>
       </c>
+      <c r="K44" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="L44" s="6" t="s">
+        <v>259</v>
+      </c>
       <c r="N44" s="11"/>
-      <c r="O44" s="11"/>
-      <c r="P44" s="11"/>
+      <c r="O44" t="s">
+        <v>260</v>
+      </c>
+      <c r="P44" t="s">
+        <v>261</v>
+      </c>
       <c r="Q44" s="11"/>
       <c r="R44" s="11"/>
       <c r="S44" s="11"/>
     </row>
     <row r="45" spans="1:19" ht="29.1">
       <c r="A45" s="1" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="C45" s="11"/>
       <c r="D45" s="1" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="N45" s="6" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="46" spans="1:19" ht="43.5">
       <c r="A46" s="1" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="C46" s="11"/>
       <c r="D46" s="1" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>80</v>
       </c>
       <c r="O46" s="6" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="P46" s="6" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="Q46" s="6" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="R46" s="6" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="47" spans="1:19" ht="43.5">
       <c r="A47" s="1" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="48" spans="1:19">
@@ -3033,7 +3067,7 @@
     <hyperlink ref="B42" r:id="rId43" display="SpagoBI" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
     <hyperlink ref="B38" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
     <hyperlink ref="B11" r:id="rId45" xr:uid="{8A8D59FF-773A-4DCE-AA54-3A9635FD2929}"/>
-    <hyperlink ref="O30" r:id="rId46" xr:uid="{1BD38749-9B8E-4D3C-B377-34495CE50767}"/>
+    <hyperlink ref="O30" r:id="rId46" display="8 GB (recommanded)" xr:uid="{1BD38749-9B8E-4D3C-B377-34495CE50767}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId47"/>

</xml_diff>